<commit_message>
Atualização automática - 2025-10-21 18:53
</commit_message>
<xml_diff>
--- a/data/custos fixos.xlsx
+++ b/data/custos fixos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvand\Desktop\Adoro Pizza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D5C8D7-69E8-462B-A44D-276608E65350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB3659-A95B-4880-B0AE-1C715D6767A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CA3ACF0-1F9C-4141-BCA0-0B81B2B0FDCA}"/>
   </bookViews>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02DCF94-AAB1-4E53-9FD7-873935BED76E}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>